<commit_message>
Adding feature files with cucumber
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/Testcase&featurefile.xlsx
+++ b/src/test/resources/TestData/Testcase&featurefile.xlsx
@@ -236,9 +236,6 @@
 Then I should see'Your message has been sent'</t>
   </si>
   <si>
-    <t>As a non register user,I should NOT be able to refer a prodcut to a friend</t>
-  </si>
-  <si>
     <t>I should NOT able to refer a prodcut to a friend when I am not registered</t>
   </si>
   <si>
@@ -266,6 +263,9 @@
 And I click on sort by
 And I select on high to low
 Then I should see price organised high to low</t>
+  </si>
+  <si>
+    <t>As a non register user,I should NOT be able to refer a product to a friend</t>
   </si>
 </sst>
 </file>
@@ -831,7 +831,7 @@
   <dimension ref="A2:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="CF6" sqref="CF6"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -889,13 +889,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="75">
@@ -903,13 +903,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>44</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -920,6 +920,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>